<commit_message>
adding new data and layout sets
</commit_message>
<xml_diff>
--- a/data/2021-09-01_geobacter_layout.xlsx
+++ b/data/2021-09-01_geobacter_layout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garc286/RStudio/stillage_general_script/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\stillage_general_script\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F66FF9-4517-F747-B0D7-8D38792DF0EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55F5E38-C3BC-418C-8140-22446DD99DA0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4000" yWindow="4160" windowWidth="28800" windowHeight="18000" xr2:uid="{318F1633-56B8-984D-8E8D-FBAE4BE2DA50}"/>
+    <workbookView xWindow="30300" yWindow="1590" windowWidth="18000" windowHeight="9360" xr2:uid="{318F1633-56B8-984D-8E8D-FBAE4BE2DA50}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="52">
   <si>
     <t>96 well plate template</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t>Fodder yeast</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -250,7 +253,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -348,11 +351,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -401,6 +415,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -723,23 +740,23 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection sqref="A1:M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="13" width="3.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="3.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="15" t="s">
         <v>36</v>
       </c>
@@ -780,7 +797,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -821,7 +838,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>3</v>
       </c>
@@ -862,7 +879,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
@@ -903,7 +920,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>5</v>
       </c>
@@ -944,7 +961,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>6</v>
       </c>
@@ -985,7 +1002,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
@@ -1026,7 +1043,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>8</v>
       </c>
@@ -1067,7 +1084,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>10</v>
       </c>
@@ -1108,7 +1125,11 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="17" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:13" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="H10" s="20" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="76" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
@@ -1123,14 +1144,14 @@
       <selection activeCell="L4" sqref="L4:L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="2">
@@ -1170,7 +1191,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1214,7 +1235,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
         <v>3</v>
@@ -1256,7 +1277,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
         <v>4</v>
@@ -1298,7 +1319,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="2" t="s">
         <v>5</v>
@@ -1340,7 +1361,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2" t="s">
         <v>6</v>
@@ -1382,7 +1403,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
         <v>7</v>
@@ -1424,7 +1445,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
         <v>8</v>
@@ -1466,7 +1487,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1510,7 +1531,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:14" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1526,7 +1547,7 @@
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C13" s="3" t="s">
         <v>33</v>
       </c>
@@ -1540,12 +1561,12 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
       <c r="H19" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C21" s="4" t="s">
         <v>11</v>
       </c>
@@ -1553,7 +1574,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C22" s="4" t="s">
         <v>13</v>
       </c>
@@ -1561,7 +1582,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C23" s="4" t="s">
         <v>14</v>
       </c>
@@ -1569,7 +1590,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C24" s="4" t="s">
         <v>15</v>
       </c>
@@ -1577,7 +1598,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C25" s="4" t="s">
         <v>16</v>
       </c>
@@ -1585,7 +1606,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C26" s="4" t="s">
         <v>17</v>
       </c>
@@ -1593,7 +1614,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C27" s="4" t="s">
         <v>18</v>
       </c>
@@ -1601,7 +1622,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C28" s="4" t="s">
         <v>19</v>
       </c>
@@ -1609,7 +1630,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="3:8" x14ac:dyDescent="0.2">
+    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C29" s="4"/>
       <c r="E29" s="4"/>
     </row>

</xml_diff>